<commit_message>
He modificado algunas respuestas del cuestionario del usuario AA que estaban mal.
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/data/meta_responses_1.xlsx
+++ b/data_analysis/db_env/app/data/meta_responses_1.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
+    <sheet r:id="rId1" sheetId="1" name="Respuestas de formulario 1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -317,21 +320,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -339,234 +344,220 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="10">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF442F65"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF5B3F86"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF442F65"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF5B3F86"/>
+        <color rgb="FF442f65"/>
       </left>
       <right style="thin">
-        <color rgb="FF5B3F86"/>
+        <color rgb="FF5b3f86"/>
       </right>
       <top style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FF442f65"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FF442f65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF5B3F86"/>
+        <color rgb="FF5b3f86"/>
       </left>
       <right style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FF5b3f86"/>
       </right>
       <top style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FF442f65"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FF442f65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FF5b3f86"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF442f65"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF442f65"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF442f65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF442f65"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
       </left>
       <right style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FFffffff"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FFffffff"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FF442f65"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFffffff"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FFffffff"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FF442f65"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFf8f9fa"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFf8f9fa"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FF442f65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFf8f9fa"/>
       </left>
       <right style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FFf8f9fa"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFf8f9fa"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FF442f65"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFf8f9fa"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442f65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFf8f9fa"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442f65"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="16">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF5B3F86"/>
-          <bgColor rgb="FF5B3F86"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F9FA"/>
-          <bgColor rgb="FFF8F9FA"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Respuestas de formulario 1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:BX3" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:BX3" displayName="Form_Responses1" name="Form_Responses1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:BX3"/>
   <tableColumns count="76">
     <tableColumn name="Marca temporal" id="1"/>
     <tableColumn name="[ID] Escribe el identificador que has escrito en la aplicación de realidad virtual. Si no sabes cuál es, pregúntale al investigador." id="2"/>
@@ -645,19 +636,19 @@
     <tableColumn name="[S-CL] Durante la tarea, ¿en qué medida se ha sentido insegur@, desalentad@, irritad@, tens@) o preocupad@ o por el contrario, se ha sentido segur@, content@, relajad@ y satisfech@?   " id="75"/>
     <tableColumn name="[EMAIL] Correo electrónico" id="76"/>
   </tableColumns>
-  <tableStyleInfo name="Respuestas de formulario 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="1" showFirstColumn="1"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -684,22 +675,82 @@
         <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -711,173 +762,266 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:BX3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.88"/>
-    <col customWidth="1" min="2" max="2" width="37.63"/>
-    <col customWidth="1" min="3" max="5" width="18.88"/>
-    <col customWidth="1" min="6" max="18" width="37.63"/>
-    <col customWidth="1" min="19" max="19" width="94.38"/>
-    <col customWidth="1" min="20" max="20" width="84.75"/>
-    <col customWidth="1" min="21" max="21" width="96.0"/>
-    <col customWidth="1" min="22" max="22" width="104.38"/>
-    <col customWidth="1" min="23" max="36" width="37.63"/>
-    <col customWidth="1" min="37" max="37" width="107.0"/>
-    <col customWidth="1" min="38" max="75" width="37.63"/>
-    <col customWidth="1" min="76" max="82" width="18.88"/>
+    <col min="1" max="1" style="13" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="15" width="43.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="15" width="44.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="15" width="104.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="15" width="103.005" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="15" width="63.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="15" width="63.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="15" width="119.005" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="15" width="107.005" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="46" max="46" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="47" max="47" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="48" max="48" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="49" max="49" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="50" max="50" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="51" max="51" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="52" max="52" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="53" max="53" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="54" max="54" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="55" max="55" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="56" max="56" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="57" max="57" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="58" max="58" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="59" max="59" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="60" max="60" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="61" max="61" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="62" max="62" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="63" max="63" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="64" max="64" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="65" max="65" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="66" max="66" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="67" max="67" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="68" max="68" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="69" max="69" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="70" max="70" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="71" max="71" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="72" max="72" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="73" max="73" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="74" max="74" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="75" max="75" style="15" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="76" max="76" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -886,7 +1030,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -925,112 +1069,112 @@
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AM1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AP1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AR1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AS1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AT1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AU1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AV1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AW1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AX1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AY1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BA1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BB1" s="3" t="s">
         <v>53</v>
       </c>
       <c r="BC1" s="2" t="s">
@@ -1078,19 +1222,19 @@
       <c r="BQ1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BR1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BS1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BT1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BU1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BV1" s="3" t="s">
         <v>73</v>
       </c>
       <c r="BW1" s="3" t="s">
@@ -1100,15 +1244,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="5">
-        <v>45587.59744890046</v>
+        <v>45587.597453703704</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="6">
-        <v>21.0</v>
+      <c r="C2" s="7">
+        <v>21</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>77</v>
@@ -1116,8 +1260,8 @@
       <c r="E2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="6">
-        <v>7.0</v>
+      <c r="F2" s="7">
+        <v>7</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>79</v>
@@ -1155,113 +1299,113 @@
       <c r="R2" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S2" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="T2" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="U2" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="V2" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="W2" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="X2" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="Y2" s="6">
-        <v>6.0</v>
-      </c>
-      <c r="Z2" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="AA2" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="AB2" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="AC2" s="6">
-        <v>6.0</v>
-      </c>
-      <c r="AD2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="AE2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="AF2" s="6">
-        <v>6.0</v>
-      </c>
-      <c r="AG2" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="AH2" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="AI2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="AJ2" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="AK2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="AL2" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="AM2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="AN2" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="AO2" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="AP2" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="AQ2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="AR2" s="6">
-        <v>6.0</v>
-      </c>
-      <c r="AS2" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="AT2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="AU2" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="AV2" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="AW2" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="AX2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="AY2" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="AZ2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="BA2" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="BB2" s="6">
-        <v>1.0</v>
+      <c r="S2" s="7">
+        <v>7</v>
+      </c>
+      <c r="T2" s="7">
+        <v>7</v>
+      </c>
+      <c r="U2" s="7">
+        <v>1</v>
+      </c>
+      <c r="V2" s="7">
+        <v>1</v>
+      </c>
+      <c r="W2" s="7">
+        <v>4</v>
+      </c>
+      <c r="X2" s="7">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="7">
+        <v>6</v>
+      </c>
+      <c r="Z2" s="7">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="7">
+        <v>6</v>
+      </c>
+      <c r="AD2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="7">
+        <v>7</v>
+      </c>
+      <c r="AF2" s="7">
+        <v>6</v>
+      </c>
+      <c r="AG2" s="7">
+        <v>7</v>
+      </c>
+      <c r="AH2" s="7">
+        <v>7</v>
+      </c>
+      <c r="AI2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AK2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="7">
+        <v>7</v>
+      </c>
+      <c r="AM2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="7">
+        <v>5</v>
+      </c>
+      <c r="AO2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AP2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AQ2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="7">
+        <v>6</v>
+      </c>
+      <c r="AS2" s="7">
+        <v>4</v>
+      </c>
+      <c r="AT2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="7">
+        <v>5</v>
+      </c>
+      <c r="AV2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AW2" s="7">
+        <v>4</v>
+      </c>
+      <c r="AX2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="7">
+        <v>4</v>
+      </c>
+      <c r="AZ2" s="7">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="7">
+        <v>5</v>
+      </c>
+      <c r="BB2" s="7">
+        <v>1</v>
       </c>
       <c r="BC2" s="6" t="s">
         <v>91</v>
@@ -1308,262 +1452,262 @@
       <c r="BQ2" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="BR2" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="BS2" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="BT2" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="BU2" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="BV2" s="6">
-        <v>9.0</v>
-      </c>
-      <c r="BW2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="BX2" s="7" t="s">
+      <c r="BR2" s="7">
+        <v>3</v>
+      </c>
+      <c r="BS2" s="7">
+        <v>7</v>
+      </c>
+      <c r="BT2" s="7">
+        <v>2</v>
+      </c>
+      <c r="BU2" s="7">
+        <v>4</v>
+      </c>
+      <c r="BV2" s="7">
+        <v>9</v>
+      </c>
+      <c r="BW2" s="7">
+        <v>1</v>
+      </c>
+      <c r="BX2" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="8">
-        <v>45590.59359730324</v>
-      </c>
-      <c r="B3" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="9">
+        <v>45590.59359953704</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="9">
-        <v>21.0</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="11">
+        <v>21</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="9">
-        <v>9.0</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="11">
+        <v>9</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="O3" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="S3" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="T3" s="9">
-        <v>7.0</v>
-      </c>
-      <c r="U3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="V3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="W3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="X3" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="Y3" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="Z3" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="AA3" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="AB3" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="AC3" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="AD3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="AE3" s="9">
-        <v>7.0</v>
-      </c>
-      <c r="AF3" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="AG3" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="AH3" s="9">
-        <v>7.0</v>
-      </c>
-      <c r="AI3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="AJ3" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="AK3" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="AL3" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="AM3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="AN3" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="AO3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="AP3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="AQ3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="AR3" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="AS3" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="AT3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="AU3" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="AV3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="AW3" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="AX3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="AY3" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="AZ3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="BA3" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="BB3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="BC3" s="9" t="s">
+      <c r="S3" s="11">
+        <v>6</v>
+      </c>
+      <c r="T3" s="11">
+        <v>7</v>
+      </c>
+      <c r="U3" s="11">
+        <v>1</v>
+      </c>
+      <c r="V3" s="11">
+        <v>1</v>
+      </c>
+      <c r="W3" s="11">
+        <v>1</v>
+      </c>
+      <c r="X3" s="11">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="11">
+        <v>5</v>
+      </c>
+      <c r="Z3" s="11">
+        <v>5</v>
+      </c>
+      <c r="AA3" s="11">
+        <v>4</v>
+      </c>
+      <c r="AB3" s="11">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="11">
+        <v>6</v>
+      </c>
+      <c r="AD3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="11">
+        <v>7</v>
+      </c>
+      <c r="AF3" s="11">
+        <v>6</v>
+      </c>
+      <c r="AG3" s="11">
+        <v>6</v>
+      </c>
+      <c r="AH3" s="11">
+        <v>7</v>
+      </c>
+      <c r="AI3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="11">
+        <v>2</v>
+      </c>
+      <c r="AK3" s="11">
+        <v>3</v>
+      </c>
+      <c r="AL3" s="11">
+        <v>6</v>
+      </c>
+      <c r="AM3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="11">
+        <v>6</v>
+      </c>
+      <c r="AO3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AP3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AR3" s="11">
+        <v>6</v>
+      </c>
+      <c r="AS3" s="11">
+        <v>4</v>
+      </c>
+      <c r="AT3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AU3" s="11">
+        <v>5</v>
+      </c>
+      <c r="AV3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="11">
+        <v>5</v>
+      </c>
+      <c r="AX3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="11">
+        <v>4</v>
+      </c>
+      <c r="AZ3" s="11">
+        <v>1</v>
+      </c>
+      <c r="BA3" s="11">
+        <v>4</v>
+      </c>
+      <c r="BB3" s="11">
+        <v>1</v>
+      </c>
+      <c r="BC3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="BD3" s="9" t="s">
+      <c r="BD3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="BE3" s="9" t="s">
+      <c r="BE3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="BF3" s="9" t="s">
+      <c r="BF3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="BG3" s="9" t="s">
+      <c r="BG3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="BH3" s="9" t="s">
+      <c r="BH3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="BI3" s="9" t="s">
+      <c r="BI3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="BJ3" s="9" t="s">
+      <c r="BJ3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="BK3" s="9" t="s">
+      <c r="BK3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="BL3" s="9" t="s">
+      <c r="BL3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="BM3" s="9" t="s">
+      <c r="BM3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="BN3" s="9" t="s">
+      <c r="BN3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="BO3" s="9" t="s">
+      <c r="BO3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="BP3" s="9" t="s">
+      <c r="BP3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="BQ3" s="9" t="s">
+      <c r="BQ3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="BR3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="BS3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="BT3" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="BU3" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="BV3" s="9">
-        <v>8.0</v>
-      </c>
-      <c r="BW3" s="9">
-        <v>8.0</v>
-      </c>
-      <c r="BX3" s="10" t="s">
+      <c r="BR3" s="11">
+        <v>1</v>
+      </c>
+      <c r="BS3" s="11">
+        <v>1</v>
+      </c>
+      <c r="BT3" s="11">
+        <v>1</v>
+      </c>
+      <c r="BU3" s="11">
+        <v>2</v>
+      </c>
+      <c r="BV3" s="11">
+        <v>8</v>
+      </c>
+      <c r="BW3" s="11">
+        <v>8</v>
+      </c>
+      <c r="BX3" s="12" t="s">
         <v>98</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>